<commit_message>
Replaced with new ATMEGA328 chip and modified PWM pins
</commit_message>
<xml_diff>
--- a/generated/BOM_BN_REV3A_Explorer_20190823_prod.xlsx
+++ b/generated/BOM_BN_REV3A_Explorer_20190823_prod.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ling\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ling\Desktop\Barnabas\barnabas-noggin\generated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{56EB2181-0E37-49B7-B76B-B04157107CBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6049E9F4-2A2B-4E69-AAAC-E908BB361F3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Barnabas Noggin rev 3A" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
   <si>
     <t>1K</t>
   </si>
@@ -460,9 +467,6 @@
     <t>No Place</t>
   </si>
   <si>
-    <t>Other Source</t>
-  </si>
-  <si>
     <t>https://www.alibaba.com/product-detail/Electronic-Components-Capacitor-Chip-Interface-Ic_62158426034.html?spm=a2700.7724838.2017115.1.c5293cfbv2l3JU&amp;s=p</t>
   </si>
   <si>
@@ -473,12 +477,45 @@
   </si>
   <si>
     <t>Total Parts</t>
+  </si>
+  <si>
+    <t>On Hand</t>
+  </si>
+  <si>
+    <t>Not Sure</t>
+  </si>
+  <si>
+    <t>From Nano</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics/CSTNE12M0G550000R0/490-17943-1-ND/8747751</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/c-k/PTS820-J15M-SMTR-LFS/CKN10506CT-ND/4176681</t>
+  </si>
+  <si>
+    <t>Purchasing</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Need to purchase</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/ATMEGA328P-MUR/ATMEGA328P-MURCT-ND/3440953</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/bourns-inc/MF-FSMF050X-2/MF-FSMF050X-2CT-ND/2039389</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/texas-instruments/LP2985-33DBVR/296-18476-1-ND/809911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -998,7 +1035,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1012,6 +1049,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1052,7 +1092,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1368,17 +1408,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.06640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="27.53125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1388,10 +1428,11 @@
     <col min="9" max="9" width="25.06640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.86328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="136.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.9296875" customWidth="1"/>
+    <col min="13" max="13" width="136.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>129</v>
       </c>
@@ -1426,10 +1467,13 @@
         <v>139</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1459,9 +1503,12 @@
         <v>1</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1491,9 +1538,12 @@
         <v>7</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L4" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1523,9 +1573,12 @@
         <v>12</v>
       </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1555,9 +1608,12 @@
         <v>18</v>
       </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L6" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1591,9 +1647,12 @@
       <c r="K7" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1623,9 +1682,12 @@
         <v>26</v>
       </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1655,9 +1717,14 @@
         <v>32</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1687,9 +1754,12 @@
         <v>39</v>
       </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1719,9 +1789,12 @@
         <v>44</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1751,9 +1824,14 @@
         <v>49</v>
       </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L12" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1787,9 +1865,12 @@
       <c r="K13" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1819,9 +1900,14 @@
         <v>56</v>
       </c>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1855,9 +1941,12 @@
       <c r="K15" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L15" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1887,11 +1976,14 @@
         <v>17</v>
       </c>
       <c r="K16" s="4"/>
-      <c r="L16" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L16" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1921,9 +2013,14 @@
         <v>67</v>
       </c>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L17" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1953,9 +2050,12 @@
         <v>73</v>
       </c>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1985,9 +2085,12 @@
         <v>79</v>
       </c>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L19" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -2021,9 +2124,12 @@
       <c r="K20" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L20" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -2057,9 +2163,12 @@
       <c r="K21" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L21" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2089,9 +2198,12 @@
         <v>88</v>
       </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L22" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2121,9 +2233,14 @@
         <v>95</v>
       </c>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2153,9 +2270,12 @@
         <v>101</v>
       </c>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L24" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2185,9 +2305,12 @@
         <v>107</v>
       </c>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2217,9 +2340,12 @@
         <v>112</v>
       </c>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2249,9 +2375,12 @@
         <v>119</v>
       </c>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L27" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2281,29 +2410,32 @@
         <v>125</v>
       </c>
       <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B30" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C30">
         <f>SUMIF(D3:D28,"Thru-Hole",F3:F28)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B31" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31">
         <f>C32-C30</f>
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B32" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32">
         <f>SUM(F3:F28)</f>
@@ -2312,7 +2444,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L16" r:id="rId1"/>
+    <hyperlink ref="L9" r:id="rId1" display="https://www.digikey.com/product-detail/en/murata-electronics/CSTNE12M0G550000R0/490-17943-1-ND/8747751" xr:uid="{8F0E13E3-A713-481B-9A08-327EE71E89A7}"/>
+    <hyperlink ref="L12" r:id="rId2" display="https://www.digikey.com/product-detail/en/c-k/PTS820-J15M-SMTR-LFS/CKN10506CT-ND/4176681" xr:uid="{40CF17AD-F570-4E72-9EE9-D0F698082B24}"/>
+    <hyperlink ref="M9" r:id="rId3" xr:uid="{FE949140-4F6B-4039-90C4-AE621D8B961A}"/>
+    <hyperlink ref="M12" r:id="rId4" xr:uid="{E53CD9C7-7434-4298-AFA1-F1CA244BAB6C}"/>
+    <hyperlink ref="M16" r:id="rId5" xr:uid="{CBA78BA5-BBA0-4BA2-ABDC-DD90EAD00EE6}"/>
+    <hyperlink ref="M14" r:id="rId6" xr:uid="{C90AD723-33F8-43A0-833C-0CFBAE433209}"/>
+    <hyperlink ref="M17" r:id="rId7" xr:uid="{18C3F64A-7B48-4386-BBA4-39C69087CC79}"/>
+    <hyperlink ref="M23" r:id="rId8" xr:uid="{3B0B471F-12E8-46E8-9D6A-B92E63FB97ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>